<commit_message>
sl added in duplicate rows
</commit_message>
<xml_diff>
--- a/reports/_APL_SUMMIT ALLIANCE PORT LIMITED (OCL)_container_report_2018-12-03_40_.xlsx
+++ b/reports/_APL_SUMMIT ALLIANCE PORT LIMITED (OCL)_container_report_2018-12-03_40_.xlsx
@@ -1309,7 +1309,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="5"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438" hidden="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="202.18988764044946" hidden="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="24.8561797752809"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="19.4561797752809"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="23.0561797752809"/>
@@ -2265,37 +2265,16 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
-      <c r="H14" s="0"/>
-      <c r="I14" s="0"/>
-      <c r="J14" s="0"/>
-      <c r="K14" s="0"/>
-      <c r="L14" s="0"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="0"/>
-      <c r="O14" s="0"/>
-      <c r="P14" s="0"/>
-      <c r="Q14" s="0"/>
-      <c r="R14" s="0"/>
-      <c r="S14" s="0"/>
-      <c r="T14" s="0"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="0"/>
-      <c r="W14" s="0"/>
-      <c r="X14" s="0" t="inlineStr">
-        <is>
-          <t>INTERIOR PANEL INK</t>
-        </is>
-      </c>
-      <c r="Y14" s="0"/>
-      <c r="Z14" s="0"/>
-      <c r="AA14" s="0"/>
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>[nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, nil, "PANELS-(PANELS)", "Right side panel -(Right side panel )", "INTERIOR PANEL INK", "", "", ""]</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="n">

</xml_diff>